<commit_message>
import limit scenario added and refactor
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Contact.xlsx
+++ b/src/test/resources/testData/Contact.xlsx
@@ -12,11 +12,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>SKU</t>
   </si>
   <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
     <t>DIA_FirstName</t>
   </si>
   <si>
@@ -32,10 +38,37 @@
     <t>İsim</t>
   </si>
   <si>
-    <t>Kişi-10</t>
-  </si>
-  <si>
-    <t>1f344eb7-5f99-4e08-a7be-055189c0e343</t>
+    <t>98592242-88ef-40ab-a01b-587ce7d54953</t>
+  </si>
+  <si>
+    <t>IWSA</t>
+  </si>
+  <si>
+    <t>efc2de0e-deb3-4acc-8409-c99866c70e31</t>
+  </si>
+  <si>
+    <t>Reserve</t>
+  </si>
+  <si>
+    <t>f5ea80f4-e1fd-44b8-ae57-fe9ad8e92b4b</t>
+  </si>
+  <si>
+    <t>e32fdcb7-c5ac-4c22-b844-f9a6f4d153f3</t>
+  </si>
+  <si>
+    <t>2f3136ba-5728-4b54-bac4-379b295ca7e6</t>
+  </si>
+  <si>
+    <t>Kişi-05</t>
+  </si>
+  <si>
+    <t>d0a831c9-f8ba-4a6c-ba24-e23ce758f086</t>
+  </si>
+  <si>
+    <t>5498381895</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -80,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -91,24 +124,90 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>